<commit_message>
finish exam button added
</commit_message>
<xml_diff>
--- a/doc.xlsx
+++ b/doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eyup\PycharmProjects\QtLoadQuestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4616664-67B1-4EEB-B312-D9C632419DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E000DABB-51FE-4488-A962-327233E651F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>JAVA</t>
-  </si>
-  <si>
-    <t>PYTHON</t>
-  </si>
-  <si>
-    <t>GOOGLE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="73">
   <si>
     <t>a</t>
   </si>
@@ -54,9 +42,6 @@
     <t>e</t>
   </si>
   <si>
-    <t>KOTLİN</t>
-  </si>
-  <si>
     <t>1.jpg</t>
   </si>
   <si>
@@ -84,129 +69,24 @@
     <t>1) Aşağıdakilerden hangisi büyüktür ya da eşittir manasına gelen karşılaştırma operatörleridir?</t>
   </si>
   <si>
-    <t>&lt;=</t>
-  </si>
-  <si>
-    <t>!=</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =&gt;</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ==</t>
-  </si>
-  <si>
     <t>2) Aşağıdakilerden hangisi bir döngü deyimi değildir?</t>
   </si>
   <si>
-    <t>if else</t>
-  </si>
-  <si>
-    <t>for</t>
-  </si>
-  <si>
-    <t>foreach</t>
-  </si>
-  <si>
-    <t>do while</t>
-  </si>
-  <si>
-    <t>while</t>
-  </si>
-  <si>
     <t>3) Hangisi kurallara uymayan bir değişken adıdır?</t>
   </si>
   <si>
-    <t>ad_soyad</t>
-  </si>
-  <si>
-    <t>ad3soyad4</t>
-  </si>
-  <si>
-    <t>ad/Soyad</t>
-  </si>
-  <si>
-    <t>adSoyad</t>
-  </si>
-  <si>
-    <t>soyadAd</t>
-  </si>
-  <si>
     <t>4) Aşağıda  verilen  değişken  ismi  ve  değerlerinden hangisi doğru tanımlanmıştır?</t>
   </si>
   <si>
-    <t>adı Soyadı=Monty Python</t>
-  </si>
-  <si>
-    <t>programAdi= Python</t>
-  </si>
-  <si>
-    <t>Doğum Yılı=1990</t>
-  </si>
-  <si>
-    <t>dogumYeri="Hollanda"</t>
-  </si>
-  <si>
-    <t>%dilimi=10</t>
-  </si>
-  <si>
     <t>5) Python'da hazırlanarak  kaydedilen  program dosyaları hangi uzantıya sahiptir?</t>
   </si>
   <si>
-    <t>.doc</t>
-  </si>
-  <si>
-    <t>.prg</t>
-  </si>
-  <si>
-    <t>.py</t>
-  </si>
-  <si>
-    <t>.px</t>
-  </si>
-  <si>
-    <t>.exe</t>
-  </si>
-  <si>
     <t>6) Aşağıda verilen for döngüsü kullanımlarının hangisinde yazım hatası vardır?</t>
   </si>
   <si>
-    <t>for x in range("Burak Bora AL"):</t>
-  </si>
-  <si>
-    <t>for x in "Burak Bora AL":</t>
-  </si>
-  <si>
-    <t>for x in range(3, 6):</t>
-  </si>
-  <si>
-    <t>for x in range(10):</t>
-  </si>
-  <si>
-    <t>for x in range(3, 8, 2):</t>
-  </si>
-  <si>
     <t>8) Python'da yazılan kodları derlemek (çalıştırmak ) için kullanılan kısayol tuşu hangisidir?</t>
   </si>
   <si>
-    <t>enter</t>
-  </si>
-  <si>
-    <t>f5</t>
-  </si>
-  <si>
-    <t>f3</t>
-  </si>
-  <si>
-    <t>del</t>
-  </si>
-  <si>
-    <t>ctrl</t>
-  </si>
-  <si>
     <t>3.jpg</t>
   </si>
   <si>
@@ -229,6 +109,141 @@
   </si>
   <si>
     <t>10.jpg</t>
+  </si>
+  <si>
+    <t>A) &lt;=</t>
+  </si>
+  <si>
+    <t>A) if else</t>
+  </si>
+  <si>
+    <t>A) ad_soyad</t>
+  </si>
+  <si>
+    <t>A) adı Soyadı=Monty Python</t>
+  </si>
+  <si>
+    <t>A) .doc</t>
+  </si>
+  <si>
+    <t>A) for x in range("Burak Bora AL"):</t>
+  </si>
+  <si>
+    <t>A) C</t>
+  </si>
+  <si>
+    <t>A) enter</t>
+  </si>
+  <si>
+    <t>A) GOOGLE</t>
+  </si>
+  <si>
+    <t>B) !=</t>
+  </si>
+  <si>
+    <t>B) for</t>
+  </si>
+  <si>
+    <t>B) ad3soyad4</t>
+  </si>
+  <si>
+    <t>B) programAdi= Python</t>
+  </si>
+  <si>
+    <t>B) .prg</t>
+  </si>
+  <si>
+    <t>B) for x in "Burak Bora AL":</t>
+  </si>
+  <si>
+    <t>B) JAVA</t>
+  </si>
+  <si>
+    <t>B) f5</t>
+  </si>
+  <si>
+    <t>B) KOTLİN</t>
+  </si>
+  <si>
+    <t>C)  =&gt;</t>
+  </si>
+  <si>
+    <t>C)  foreach</t>
+  </si>
+  <si>
+    <t>C)  ad/Soyad</t>
+  </si>
+  <si>
+    <t>C)  Doğum Yılı=1990</t>
+  </si>
+  <si>
+    <t>C)  .py</t>
+  </si>
+  <si>
+    <t>C)  for x in range(3, 6):</t>
+  </si>
+  <si>
+    <t>C)  PYTHON</t>
+  </si>
+  <si>
+    <t>C)  f3</t>
+  </si>
+  <si>
+    <t>C)  C</t>
+  </si>
+  <si>
+    <t>D)  &gt;=</t>
+  </si>
+  <si>
+    <t>D)  do while</t>
+  </si>
+  <si>
+    <t>D)  adSoyad</t>
+  </si>
+  <si>
+    <t>D)  dogumYeri="Hollanda"</t>
+  </si>
+  <si>
+    <t>D)  .px</t>
+  </si>
+  <si>
+    <t>D)  for x in range(10):</t>
+  </si>
+  <si>
+    <t>D)  GOOGLE</t>
+  </si>
+  <si>
+    <t>D)  del</t>
+  </si>
+  <si>
+    <t>D)  JAVA</t>
+  </si>
+  <si>
+    <t>E) while</t>
+  </si>
+  <si>
+    <t>E) soyadAd</t>
+  </si>
+  <si>
+    <t>E) %dilimi=10</t>
+  </si>
+  <si>
+    <t>E) .exe</t>
+  </si>
+  <si>
+    <t>E) for x in range(3, 8, 2):</t>
+  </si>
+  <si>
+    <t>E) KOTLİN</t>
+  </si>
+  <si>
+    <t>E) ctrl</t>
+  </si>
+  <si>
+    <t>E) GOOGLE</t>
+  </si>
+  <si>
+    <t>E)  ==</t>
   </si>
 </sst>
 </file>
@@ -558,7 +573,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,288 +589,288 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="G4" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="H7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
         <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" t="s">
         <v>3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>